<commit_message>
update of feature list
</commit_message>
<xml_diff>
--- a/Documents/FeatureList -/Feature List.xlsx
+++ b/Documents/FeatureList -/Feature List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20350"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\student\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\Computing-Project-2019---PathFinder\Documents\FeatureList -\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50D2267F-6BFC-437F-B245-E1FEEDF08C32}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CA7DDD7-934A-4089-9581-768553A7F7D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="7650" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sprints" sheetId="1" r:id="rId1"/>
@@ -21,12 +21,18 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="72">
   <si>
     <t>Feature</t>
   </si>
@@ -81,9 +87,6 @@
 </t>
   </si>
   <si>
-    <t>Marker to display where you are</t>
-  </si>
-  <si>
     <t>Application - Map Marker</t>
   </si>
   <si>
@@ -162,13 +165,92 @@
     <t>Hosted site - implementation of database onto site</t>
   </si>
   <si>
-    <t>Organisations send in registeration request - used to create org in database</t>
-  </si>
-  <si>
-    <t>Present landing screen to user and request initial input (BT, NFC, QR , BC)</t>
-  </si>
-  <si>
-    <t>Possibility to update maker as user moves around</t>
+    <t>Organisations send in registeration request - used to create orginisation in database</t>
+  </si>
+  <si>
+    <t>Present landing screen to user</t>
+  </si>
+  <si>
+    <t>Marker to display where your current location is</t>
+  </si>
+  <si>
+    <t>Potentially Track User location</t>
+  </si>
+  <si>
+    <t>Hours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Responsible </t>
+  </si>
+  <si>
+    <t>Responsible</t>
+  </si>
+  <si>
+    <t>Design a website that displays information about the application and menus for the different aspects</t>
+  </si>
+  <si>
+    <t>Purple for Finished:
+Yellow for Unfinished:</t>
+  </si>
+  <si>
+    <t>the user will be shown a path using a real time icon or a series of steps during each milestone</t>
+  </si>
+  <si>
+    <t>User will be constantly detected using bluetooth beacon or will only be detected when reached a milestone</t>
+  </si>
+  <si>
+    <t>The map will display a icon that the user will click or a dropdown-menu where all locations on the map are listed</t>
+  </si>
+  <si>
+    <t>The map will display a 2d version of the building</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Display Path using shorted route algorithim </t>
+  </si>
+  <si>
+    <t>keep track of the users current progress on path</t>
+  </si>
+  <si>
+    <t>Send user new instructions when milestone reached</t>
+  </si>
+  <si>
+    <t>Notify user when destination reached</t>
+  </si>
+  <si>
+    <t>when user has reached a destination the nfc tag will send information to the user</t>
+  </si>
+  <si>
+    <t>Display Icon on map or use drop down menu where all locations are listed</t>
+  </si>
+  <si>
+    <t>Application - Route lnstructions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Database - Design </t>
+  </si>
+  <si>
+    <t>Design Database to handle website data and application data</t>
+  </si>
+  <si>
+    <t>Kevin</t>
+  </si>
+  <si>
+    <t>Kate</t>
+  </si>
+  <si>
+    <t>Chris</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kevin </t>
+  </si>
+  <si>
+    <t>Kate,Chris,Kevin</t>
+  </si>
+  <si>
+    <t>Present landing screen to user with information about the using the application</t>
+  </si>
+  <si>
+    <t>Chris,Kate</t>
   </si>
 </sst>
 </file>
@@ -228,7 +310,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -264,11 +346,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
@@ -306,22 +425,51 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -607,27 +755,27 @@
   </sheetPr>
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.140625" customWidth="1"/>
-    <col min="2" max="2" width="25.28515625" customWidth="1"/>
-    <col min="3" max="3" width="25.42578125" customWidth="1"/>
-    <col min="4" max="4" width="24.42578125" customWidth="1"/>
-    <col min="5" max="5" width="19.7109375" customWidth="1"/>
+    <col min="1" max="1" width="20.109375" customWidth="1"/>
+    <col min="2" max="2" width="25.33203125" customWidth="1"/>
+    <col min="3" max="3" width="25.44140625" customWidth="1"/>
+    <col min="4" max="4" width="24.44140625" customWidth="1"/>
+    <col min="5" max="5" width="19.6640625" customWidth="1"/>
     <col min="6" max="6" width="25" customWidth="1"/>
-    <col min="7" max="7" width="28.42578125" customWidth="1"/>
+    <col min="7" max="7" width="28.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>15</v>
@@ -636,99 +784,101 @@
         <v>16</v>
       </c>
       <c r="E1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="5" t="s">
-        <v>19</v>
-      </c>
       <c r="G1" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="12" t="s">
         <v>34</v>
-      </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12" t="s">
-        <v>35</v>
       </c>
       <c r="D2" s="12"/>
       <c r="E2" s="12"/>
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
     </row>
-    <row r="3" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>45</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
     </row>
-    <row r="4" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
     </row>
-    <row r="5" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="2" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>5</v>
       </c>
@@ -739,11 +889,11 @@
         <v>46</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>6</v>
       </c>
@@ -752,11 +902,11 @@
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>8</v>
       </c>
@@ -765,11 +915,11 @@
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>9</v>
       </c>
@@ -780,11 +930,11 @@
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>10</v>
       </c>
@@ -795,7 +945,7 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>11</v>
       </c>
@@ -806,7 +956,7 @@
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>12</v>
       </c>
@@ -817,7 +967,7 @@
       <c r="F13" s="10"/>
       <c r="G13" s="10"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>13</v>
       </c>
@@ -828,7 +978,7 @@
       <c r="F14" s="8"/>
       <c r="G14" s="10"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>14</v>
       </c>
@@ -839,9 +989,9 @@
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
@@ -850,9 +1000,9 @@
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
@@ -869,110 +1019,315 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F018BBFD-6BA3-4F99-AC1B-306B5C899706}">
-  <dimension ref="B1:Q9"/>
+  <dimension ref="A1:U11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="5.7109375" customWidth="1"/>
-    <col min="3" max="3" width="4.42578125" customWidth="1"/>
+    <col min="1" max="1" width="27.21875" customWidth="1"/>
+    <col min="2" max="2" width="5.6640625" customWidth="1"/>
+    <col min="3" max="3" width="4.44140625" customWidth="1"/>
     <col min="4" max="4" width="30" customWidth="1"/>
-    <col min="17" max="17" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.88671875" customWidth="1"/>
+    <col min="7" max="7" width="30.5546875" customWidth="1"/>
+    <col min="8" max="9" width="17.21875" customWidth="1"/>
+    <col min="10" max="10" width="34.109375" customWidth="1"/>
+    <col min="12" max="12" width="14" customWidth="1"/>
+    <col min="13" max="13" width="34" customWidth="1"/>
+    <col min="14" max="14" width="13.21875" customWidth="1"/>
+    <col min="15" max="15" width="13.88671875" customWidth="1"/>
+    <col min="16" max="16" width="33.109375" customWidth="1"/>
+    <col min="17" max="17" width="11.21875" customWidth="1"/>
+    <col min="18" max="18" width="14.77734375" customWidth="1"/>
+    <col min="19" max="19" width="31.77734375" customWidth="1"/>
+    <col min="20" max="20" width="10.5546875" customWidth="1"/>
+    <col min="21" max="21" width="13.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B1" s="13" t="s">
+    <row r="1" spans="1:21" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-    </row>
-    <row r="2" spans="2:17" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="14" t="s">
+      <c r="C1" s="24"/>
+      <c r="D1" s="25"/>
+      <c r="E1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="H1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" t="s">
+        <v>47</v>
+      </c>
+      <c r="L1" t="s">
+        <v>49</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" t="s">
+        <v>47</v>
+      </c>
+      <c r="O1" t="s">
+        <v>49</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>47</v>
+      </c>
+      <c r="R1" t="s">
+        <v>49</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="T1" t="s">
+        <v>47</v>
+      </c>
+      <c r="U1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" ht="90" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="21"/>
+      <c r="D2" s="22"/>
+      <c r="F2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="I2" t="s">
+        <v>65</v>
+      </c>
+      <c r="J2" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="M2" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="P2" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="S2" s="12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-    </row>
-    <row r="3" spans="2:17" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="15" t="s">
+      <c r="C3" s="19"/>
+      <c r="D3" s="18"/>
+      <c r="F3" t="s">
+        <v>66</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I3" t="s">
+        <v>69</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="L3" t="s">
+        <v>67</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="O3" t="s">
+        <v>65</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="R3" t="s">
+        <v>67</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="U3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" ht="52.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="13"/>
+      <c r="C4" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3">
-        <f>E4+E5+E8+E9</f>
-        <v>192</v>
-      </c>
-      <c r="P3">
-        <f>E3+F3+G3+H3</f>
-        <v>192</v>
-      </c>
-      <c r="Q3" t="str">
-        <f>IF(P3&gt;160, "Error - out of scope", "Within Scope")</f>
-        <v>Error - out of scope</v>
-      </c>
-    </row>
-    <row r="4" spans="2:17" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="16"/>
-      <c r="C4" s="15" t="s">
+      <c r="D4" s="18"/>
+      <c r="F4" t="s">
+        <v>66</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I4" t="s">
+        <v>69</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L4" t="s">
+        <v>65</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="O4" t="s">
+        <v>67</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="R4" t="s">
+        <v>66</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="U4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="13"/>
+      <c r="C5" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="D4" s="15"/>
-    </row>
-    <row r="5" spans="2:17" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="16"/>
-      <c r="C5" s="15" t="s">
+      <c r="D5" s="18"/>
+      <c r="F5" t="s">
+        <v>65</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I5" t="s">
+        <v>68</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L5" t="s">
+        <v>71</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="O5" t="s">
+        <v>66</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="R5" t="s">
+        <v>65</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="U5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" ht="46.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" t="s">
+        <v>66</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I6" t="s">
+        <v>65</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="R6" t="s">
+        <v>65</v>
+      </c>
+      <c r="S6" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="U6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="D5" s="15"/>
-      <c r="E5">
-        <f>E6+E7</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="2:17" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="E6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="2:17" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="E7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="2:17" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="16"/>
-      <c r="C8" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="18"/>
-      <c r="E8">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="2:17" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="16"/>
-      <c r="C9" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" s="18"/>
-      <c r="E9">
-        <v>170</v>
-      </c>
+      <c r="F7" t="s">
+        <v>65</v>
+      </c>
+      <c r="P7" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="R7" t="s">
+        <v>66</v>
+      </c>
+      <c r="S7" s="29"/>
+    </row>
+    <row r="8" spans="1:21" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="13"/>
+      <c r="C8" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="16"/>
+      <c r="F8" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q8" s="27"/>
+    </row>
+    <row r="9" spans="1:21" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="13"/>
+      <c r="C9" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="16"/>
+      <c r="F9" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q9" s="27"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="Q10" s="27"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="Q11" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -985,10 +1340,26 @@
     <mergeCell ref="C8:D8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003346250C7A7DC444B5B8BD6B4F11346C" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7778cca334f7cd03e5491b75ee9e5f9d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="e86b558f-1821-4180-8c71-7e32b468d584" xmlns:ns4="bb0fba86-f7fb-46c6-8423-a0b803871f4b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bb87653dc2dcaf3360c4fa507c3fae27" ns3:_="" ns4:_="">
     <xsd:import namespace="e86b558f-1821-4180-8c71-7e32b468d584"/>
@@ -1191,22 +1562,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{075B829B-61F4-43B3-99CC-BA34C4B610D0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="bb0fba86-f7fb-46c6-8423-a0b803871f4b"/>
+    <ds:schemaRef ds:uri="e86b558f-1821-4180-8c71-7e32b468d584"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8A0D4D9-C37D-4EC8-999A-605D60E3B106}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3817E717-5FBF-47BC-9D93-FE77C9207156}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1223,29 +1604,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8A0D4D9-C37D-4EC8-999A-605D60E3B106}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{075B829B-61F4-43B3-99CC-BA34C4B610D0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="bb0fba86-f7fb-46c6-8423-a0b803871f4b"/>
-    <ds:schemaRef ds:uri="e86b558f-1821-4180-8c71-7e32b468d584"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>